<commit_message>
Corrección a un recurso incorrecto
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion04/ESCALETA_CN_09_04_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion04/ESCALETA_CN_09_04_CO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="255">
   <si>
     <t>Asignatura</t>
   </si>
@@ -443,9 +443,6 @@
     <t xml:space="preserve">Se debe hacer un texto con los términos taxa, taxón, análogos, homólogos y binomial. Expandir si se quiere. </t>
   </si>
   <si>
-    <t>Se hace una imagen que englobe las distintas categorías taxonómicas; puede ser en forma de circulos, uno dentro de otro, por ejemplo. Los círculos hablan de dominio, reino, filo/división, clase, orden, familia, género y especie. Con el botón de información se explica que esta es una estructura jerarquica, y lo que haga falta para entender el recurso. En cada categoría, se pone como ejemplo la clasificación del ser humano (por ejemplo, familia hominidae, phylum chordata, etc.). En la aprte de especie se debe hacer énfasis en la importancia de esta categoría, y explicar que es dificil definirla, pues la definición más común sólo aplica para organismos con reproducción sexual. Decir que se está trabajando aún en eso.</t>
-  </si>
-  <si>
     <t>¿Cómo se organizan los taxones?</t>
   </si>
   <si>
@@ -461,18 +458,12 @@
     <t xml:space="preserve">Los tres dominios de la naturaleza </t>
   </si>
   <si>
-    <t>Las palabras de la sopa de letras don dominio, reino, filo, división, clase, orden, familia, género y especie</t>
-  </si>
-  <si>
     <t>Los dominios de la naturaleza</t>
   </si>
   <si>
     <t>Interactivo que explica los tres dominios de la naturaleza</t>
   </si>
   <si>
-    <t>Actividad acerca del dominio Archaea</t>
-  </si>
-  <si>
     <t>Eukarya: el dominio eucariota</t>
   </si>
   <si>
@@ -660,9 +651,6 @@
   </si>
   <si>
     <t>Actividad acerca de la jerarquía de los taxones</t>
-  </si>
-  <si>
-    <t>¿A qué taxones perteneces estos organismos?</t>
   </si>
   <si>
     <t>Interactivo que expone los modelos tradicional y moderno de clasificación biológica</t>
@@ -739,9 +727,6 @@
   </si>
   <si>
     <t>Recurso M15A-02</t>
-  </si>
-  <si>
-    <t>Recurso M10A-03</t>
   </si>
   <si>
     <t>Mediante este recurso se presenta un panorama histórico de la clasificación biológica, haciendo énfasis en sus representantes y las contribuciones de cada uno de ellos. Los botones de la izquierda hablan sobre: • Aristóteles (384 a.C.) • Carlos Linneo (1707 – 1778) • Erns Haeckel (1834 – 1919) • Herbert Copeland (1902 – 1968) • Robert Whittaker (1920 – 1980) • Lynn Margulis (1938 – 2011) • Carl Woese (1928 – 2012)</t>
@@ -1081,6 +1066,25 @@
   </si>
   <si>
     <t>La primera ficha explica qué es la clasificación biológica y por qué es importante. Segunda ficha explica el modelo tradicional de clasificación, con procariotas y eucariotas, y 5 reinos incluyendo el mónera. La tercera ficha explica los 3 dominios, con un reino cada uno de los dos primeros y con 4 reinos el eucariota. Se debe explicar que Archaea es en latín y arquea en español, lo mismo para Eukarya y Fungi.</t>
+  </si>
+  <si>
+    <t>Se hace una imagen que englobe las distintas categorías taxonómicas; puede ser en forma de circulos, uno dentro de otro, por ejemplo. Los círculos hablan de dominio, reino, filo/división, clase, orden, familia, género y especie. Con el botón de información se explica que esta es una estructura jerarquica, y lo que haga falta para entender el recurso. En cada categoría, se pone como ejemplo la clasificación del ser humano (por ejemplo, familia hominidae, phylum chordata, etc.). En la parte de especie se debe hacer énfasis en la importancia de esta categoría, y explicar que es dificil definirla, pues la definición más común sólo aplica para organismos con reproducción sexual. Decir que se está trabajando aún en eso.</t>
+  </si>
+  <si>
+    <r>
+      <t>Actividad acerca del dominio</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Archaea</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1398,25 +1402,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1441,6 +1433,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3708,10 +3712,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U111"/>
+  <dimension ref="A1:U110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3739,94 +3743,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="44" t="s">
+      <c r="N1" s="52"/>
+      <c r="O1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="43" t="s">
+      <c r="P1" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="45" t="s">
+      <c r="Q1" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="S1" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="U1" s="55" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="52"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="48"/>
       <c r="M2" s="13" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="55"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -3839,14 +3843,14 @@
         <v>123</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E3" s="38" t="s">
         <v>124</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="35" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H3" s="34">
         <v>1</v>
@@ -3855,7 +3859,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="41" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="K3" s="21" t="s">
         <v>20</v>
@@ -3868,7 +3872,7 @@
       </c>
       <c r="N3" s="22"/>
       <c r="O3" s="23" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P3" s="39" t="s">
         <v>19</v>
@@ -3877,16 +3881,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="S3" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="T3" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="U3" s="24" t="s">
         <v>183</v>
-      </c>
-      <c r="S3" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="T3" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="U3" s="24" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3900,14 +3904,14 @@
         <v>123</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F4" s="27"/>
       <c r="G4" s="28" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="H4" s="27">
         <v>2</v>
@@ -3938,16 +3942,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="S4" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="T4" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="U4" s="30" t="s">
         <v>191</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="T4" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="U4" s="30" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3961,14 +3965,14 @@
         <v>123</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="28" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H5" s="27">
         <v>3</v>
@@ -3990,7 +3994,7 @@
       </c>
       <c r="N5" s="22"/>
       <c r="O5" s="33" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="P5" s="39" t="s">
         <v>19</v>
@@ -3999,16 +4003,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="S5" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="T5" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="U5" s="30" t="s">
         <v>183</v>
-      </c>
-      <c r="S5" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="T5" s="32" t="s">
-        <v>187</v>
-      </c>
-      <c r="U5" s="30" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4022,14 +4026,14 @@
         <v>123</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>130</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="28" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H6" s="27">
         <v>4</v>
@@ -4051,7 +4055,7 @@
         <v>52</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="P6" s="39" t="s">
         <v>19</v>
@@ -4060,16 +4064,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="S6" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="T6" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="U6" s="30" t="s">
         <v>191</v>
-      </c>
-      <c r="S6" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="T6" s="32" t="s">
-        <v>193</v>
-      </c>
-      <c r="U6" s="30" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4121,16 +4125,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="S7" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="T7" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="U7" s="30" t="s">
         <v>183</v>
-      </c>
-      <c r="S7" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="T7" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="U7" s="30" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4151,7 +4155,7 @@
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="28" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H8" s="27">
         <v>6</v>
@@ -4160,7 +4164,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>20</v>
@@ -4182,16 +4186,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="S8" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="T8" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="U8" s="30" t="s">
         <v>191</v>
-      </c>
-      <c r="S8" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="T8" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="U8" s="30" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4212,7 +4216,7 @@
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H9" s="27">
         <v>7</v>
@@ -4221,7 +4225,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>20</v>
@@ -4234,7 +4238,7 @@
       </c>
       <c r="N9" s="22"/>
       <c r="O9" s="27" t="s">
-        <v>140</v>
+        <v>253</v>
       </c>
       <c r="P9" s="39" t="s">
         <v>19</v>
@@ -4243,16 +4247,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="S9" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="T9" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="U9" s="30" t="s">
         <v>183</v>
-      </c>
-      <c r="S9" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="T9" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="U9" s="30" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4273,7 +4277,7 @@
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="28" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H10" s="27">
         <v>8</v>
@@ -4282,7 +4286,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>20</v>
@@ -4295,7 +4299,7 @@
         <v>45</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="P10" s="39" t="s">
         <v>19</v>
@@ -4304,16 +4308,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="U10" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T10" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4336,16 +4340,16 @@
         <v>138</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="H11" s="27">
+        <v>178</v>
+      </c>
+      <c r="H11" s="34">
         <v>9</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>19</v>
@@ -4356,25 +4360,25 @@
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
       <c r="O11" s="27" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="P11" s="39" t="s">
         <v>19</v>
       </c>
       <c r="Q11" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="R11" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="S11" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="T11" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="R11" s="31" t="s">
+      <c r="U11" s="30" t="s">
         <v>179</v>
-      </c>
-      <c r="S11" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="T11" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="U11" s="30" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4397,7 +4401,7 @@
         <v>138</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>213</v>
+        <v>142</v>
       </c>
       <c r="H12" s="27">
         <v>10</v>
@@ -4406,7 +4410,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="29" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="K12" s="21" t="s">
         <v>20</v>
@@ -4416,28 +4420,28 @@
       </c>
       <c r="M12" s="22"/>
       <c r="N12" s="22" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="O12" s="27" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
       <c r="P12" s="39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q12" s="6">
         <v>6</v>
       </c>
       <c r="R12" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="U12" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S12" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T12" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="U12" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4454,13 +4458,11 @@
         <v>131</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>138</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="F13" s="27"/>
       <c r="G13" s="28" t="s">
-        <v>143</v>
+        <v>224</v>
       </c>
       <c r="H13" s="27">
         <v>11</v>
@@ -4469,7 +4471,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="29" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>20</v>
@@ -4479,28 +4481,28 @@
       </c>
       <c r="M13" s="22"/>
       <c r="N13" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="O13" s="27" t="s">
-        <v>217</v>
+        <v>52</v>
+      </c>
+      <c r="O13" s="42" t="s">
+        <v>219</v>
       </c>
       <c r="P13" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q13" s="6">
         <v>6</v>
       </c>
       <c r="R13" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T13" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="U13" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S13" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T13" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="U13" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4514,36 +4516,34 @@
         <v>123</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28" t="s">
-        <v>228</v>
+        <v>144</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="H14" s="27">
         <v>12</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="29" t="s">
-        <v>135</v>
+        <v>19</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="K14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="O14" s="42" t="s">
-        <v>223</v>
+      <c r="L14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N14" s="12"/>
+      <c r="O14" s="14" t="s">
+        <v>251</v>
       </c>
       <c r="P14" s="39" t="s">
         <v>19</v>
@@ -4552,16 +4552,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>195</v>
+        <v>236</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4575,34 +4575,36 @@
         <v>123</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>144</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="F15" s="14"/>
       <c r="G15" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="H15" s="27">
+        <v>242</v>
+      </c>
+      <c r="H15" s="34">
         <v>13</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>148</v>
+        <v>243</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M15" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="N15" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="O15" s="14" t="s">
-        <v>256</v>
+        <v>155</v>
       </c>
       <c r="P15" s="39" t="s">
         <v>19</v>
@@ -4611,16 +4613,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4634,14 +4636,14 @@
         <v>123</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="H16" s="27">
         <v>14</v>
@@ -4650,7 +4652,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="K16" s="21" t="s">
         <v>20</v>
@@ -4663,7 +4665,7 @@
         <v>27</v>
       </c>
       <c r="O16" s="14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="P16" s="39" t="s">
         <v>19</v>
@@ -4672,16 +4674,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="U16" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S16" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T16" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="U16" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4695,14 +4697,14 @@
         <v>123</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
@@ -4711,7 +4713,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>149</v>
+        <v>245</v>
       </c>
       <c r="K17" s="21" t="s">
         <v>20</v>
@@ -4724,7 +4726,7 @@
         <v>27</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="P17" s="39" t="s">
         <v>19</v>
@@ -4733,16 +4735,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S17" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="U17" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S17" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T17" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="U17" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4756,14 +4758,14 @@
         <v>123</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="3" t="s">
-        <v>249</v>
+        <v>150</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
@@ -4772,7 +4774,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>250</v>
+        <v>151</v>
       </c>
       <c r="K18" s="21" t="s">
         <v>20</v>
@@ -4782,28 +4784,28 @@
       </c>
       <c r="M18" s="12"/>
       <c r="N18" s="12" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="P18" s="39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q18" s="6">
         <v>6</v>
       </c>
       <c r="R18" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="U18" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S18" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T18" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="U18" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4817,23 +4819,23 @@
         <v>123</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H19" s="27">
+        <v>225</v>
+      </c>
+      <c r="H19" s="34">
         <v>17</v>
       </c>
       <c r="I19" s="19" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>20</v>
@@ -4843,28 +4845,28 @@
       </c>
       <c r="M19" s="12"/>
       <c r="N19" s="12" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="P19" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q19" s="6">
         <v>6</v>
       </c>
       <c r="R19" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S19" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="U19" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S19" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T19" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="U19" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4878,36 +4880,34 @@
         <v>123</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>130</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="E20" s="2"/>
       <c r="F20" s="14"/>
       <c r="G20" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H20" s="27">
         <v>18</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>155</v>
+        <v>246</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12" t="s">
-        <v>52</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="N20" s="12"/>
       <c r="O20" s="14" t="s">
-        <v>156</v>
+        <v>228</v>
       </c>
       <c r="P20" s="39" t="s">
         <v>19</v>
@@ -4916,16 +4916,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="S20" s="6" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4939,34 +4939,36 @@
         <v>123</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E21" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="F21" s="14"/>
       <c r="G21" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="H21" s="34">
+        <v>247</v>
+      </c>
+      <c r="H21" s="27">
         <v>19</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K21" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M21" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="N21" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="O21" s="14" t="s">
-        <v>232</v>
+        <v>163</v>
       </c>
       <c r="P21" s="39" t="s">
         <v>19</v>
@@ -4975,16 +4977,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="S21" s="6" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="U21" s="6" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4998,14 +5000,14 @@
         <v>123</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H22" s="27">
         <v>20</v>
@@ -5014,7 +5016,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>20</v>
@@ -5027,7 +5029,7 @@
         <v>32</v>
       </c>
       <c r="O22" s="14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="P22" s="39" t="s">
         <v>19</v>
@@ -5036,16 +5038,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="U22" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S22" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T22" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5059,23 +5061,23 @@
         <v>123</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="H23" s="27">
+        <v>162</v>
+      </c>
+      <c r="H23" s="34">
         <v>21</v>
       </c>
       <c r="I23" s="19" t="s">
         <v>20</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>255</v>
+        <v>161</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>20</v>
@@ -5085,10 +5087,10 @@
       </c>
       <c r="M23" s="12"/>
       <c r="N23" s="12" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="P23" s="39" t="s">
         <v>19</v>
@@ -5097,16 +5099,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="U23" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S23" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T23" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="U23" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5120,14 +5122,14 @@
         <v>123</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="3" t="s">
-        <v>165</v>
+        <v>226</v>
       </c>
       <c r="H24" s="27">
         <v>22</v>
@@ -5136,7 +5138,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>20</v>
@@ -5146,10 +5148,10 @@
       </c>
       <c r="M24" s="12"/>
       <c r="N24" s="12" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="O24" s="14" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="P24" s="39" t="s">
         <v>19</v>
@@ -5158,16 +5160,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="U24" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S24" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T24" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="U24" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5181,14 +5183,12 @@
         <v>123</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>130</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="E25" s="2"/>
       <c r="F25" s="14"/>
       <c r="G25" s="3" t="s">
-        <v>230</v>
+        <v>165</v>
       </c>
       <c r="H25" s="27">
         <v>23</v>
@@ -5197,7 +5197,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K25" s="21" t="s">
         <v>20</v>
@@ -5207,10 +5207,10 @@
       </c>
       <c r="M25" s="12"/>
       <c r="N25" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="O25" s="14" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="P25" s="39" t="s">
         <v>19</v>
@@ -5219,16 +5219,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="U25" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S25" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T25" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="U25" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5242,12 +5242,12 @@
         <v>123</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="14"/>
       <c r="G26" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
@@ -5256,7 +5256,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>20</v>
@@ -5269,7 +5269,7 @@
         <v>54</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="P26" s="39" t="s">
         <v>19</v>
@@ -5278,16 +5278,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S26" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="U26" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S26" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T26" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="U26" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5301,12 +5301,12 @@
         <v>123</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="14"/>
       <c r="G27" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H27" s="34">
         <v>25</v>
@@ -5315,7 +5315,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>173</v>
+        <v>214</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>20</v>
@@ -5328,7 +5328,7 @@
         <v>54</v>
       </c>
       <c r="O27" s="14" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="P27" s="39" t="s">
         <v>19</v>
@@ -5337,16 +5337,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S27" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T27" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="U27" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="S27" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T27" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="U27" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5360,12 +5360,12 @@
         <v>123</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="14"/>
       <c r="G28" s="3" t="s">
-        <v>174</v>
+        <v>10</v>
       </c>
       <c r="H28" s="27">
         <v>26</v>
@@ -5374,39 +5374,25 @@
         <v>20</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M28" s="12"/>
-      <c r="N28" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="O28" s="14" t="s">
-        <v>224</v>
-      </c>
+      <c r="N28" s="12"/>
+      <c r="O28" s="14"/>
       <c r="P28" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="6">
-        <v>6</v>
-      </c>
-      <c r="R28" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="S28" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T28" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="U28" s="6" t="s">
-        <v>194</v>
-      </c>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="6"/>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
@@ -5419,39 +5405,51 @@
         <v>123</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="14"/>
       <c r="G29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" s="34">
+        <v>216</v>
+      </c>
+      <c r="H29" s="27">
         <v>27</v>
       </c>
       <c r="I29" s="19" t="s">
         <v>20</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L29" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
+      <c r="N29" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="O29" s="14"/>
       <c r="P29" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="6"/>
+      <c r="Q29" s="6">
+        <v>6</v>
+      </c>
+      <c r="R29" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S29" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T29" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="U29" s="6" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
@@ -5464,12 +5462,12 @@
         <v>123</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="14"/>
       <c r="G30" s="3" t="s">
-        <v>220</v>
+        <v>173</v>
       </c>
       <c r="H30" s="27">
         <v>28</v>
@@ -5478,7 +5476,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>233</v>
+        <v>174</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>20</v>
@@ -5488,272 +5486,221 @@
       </c>
       <c r="M30" s="12"/>
       <c r="N30" s="12" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="O30" s="14"/>
       <c r="P30" s="39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q30" s="6">
         <v>6</v>
       </c>
       <c r="R30" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S30" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="T30" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="U30" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="S30" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T30" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="U30" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H31" s="27">
-        <v>29</v>
-      </c>
-      <c r="I31" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="K31" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="L31" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="O31" s="14"/>
-      <c r="P31" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q31" s="6">
-        <v>6</v>
-      </c>
-      <c r="R31" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="S31" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="T31" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="U31" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
         <v>117</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5768,16 +5715,10 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I31 P3:P31">
-      <formula1>$D$38:$D$39</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P30 I3:I30">
+      <formula1>$D$37:$D$38</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5789,31 +5730,31 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N31</xm:sqref>
+          <xm:sqref>N3:N30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A31</xm:sqref>
+          <xm:sqref>A3:A30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K31</xm:sqref>
+          <xm:sqref>K3:K30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L31</xm:sqref>
+          <xm:sqref>L3:L30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M31</xm:sqref>
+          <xm:sqref>M3:M30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Corrección nombre de recurso
Para que no coincida con nombre de sección
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion04/ESCALETA_CN_09_04_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion04/ESCALETA_CN_09_04_CO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="260">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1097,6 +1097,9 @@
   </si>
   <si>
     <t>Actividad  para clasificar organismos y afianzar la comprensión del concepto de categoría taxonómica</t>
+  </si>
+  <si>
+    <t>¿Qué es la taxonomía?</t>
   </si>
 </sst>
 </file>
@@ -1414,13 +1417,25 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1445,18 +1460,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3726,8 +3729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3755,94 +3758,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="45" t="s">
+      <c r="N1" s="56"/>
+      <c r="O1" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="54" t="s">
+      <c r="P1" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="55" t="s">
+      <c r="Q1" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="55" t="s">
+      <c r="S1" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="56" t="s">
+      <c r="T1" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="55" t="s">
+      <c r="U1" s="45" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="48"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="13" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="55"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="45"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -4106,7 +4109,7 @@
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="28" t="s">
-        <v>131</v>
+        <v>259</v>
       </c>
       <c r="H7" s="34">
         <v>5</v>
@@ -5990,12 +5993,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -6010,6 +6007,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P31 I3:I31">

</xml_diff>